<commit_message>
Updated mean accel hab and mean accel hab and season
</commit_message>
<xml_diff>
--- a/results/summary-means/mean_accel_habitat.xlsx
+++ b/results/summary-means/mean_accel_habitat.xlsx
@@ -1,65 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\summary-means\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4595DD36-5513-45A1-AF4C-F4F4B2805294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
-  <si>
-    <t>common_name_e</t>
-  </si>
-  <si>
-    <t>habitat_type</t>
-  </si>
-  <si>
-    <t>accel</t>
-  </si>
-  <si>
-    <t>sem</t>
-  </si>
-  <si>
-    <t>Largemouth Bass</t>
-  </si>
-  <si>
-    <t>Deep/Low SAV</t>
-  </si>
-  <si>
-    <t>Exposed/Low SAV</t>
-  </si>
-  <si>
-    <t>Mod/Dense SAV</t>
-  </si>
-  <si>
-    <t>Shallow/Dense SAV</t>
-  </si>
-  <si>
-    <t>Shallow/Low SAV</t>
-  </si>
-  <si>
-    <t>Northern Pike</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">common_name_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largemouth Bass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep/Low SAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exposed/Low SAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mod/Dense SAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow/Dense SAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow/Low SAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Pike</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,15 +88,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -385,20 +369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,170 +390,172 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>0.4</v>
       </c>
-      <c r="D2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>0.74</v>
       </c>
-      <c r="D3">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="n">
+        <v>0.042</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>0.82</v>
       </c>
-      <c r="D4">
-        <v>4.1000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="n">
+        <v>0.041</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>0.34</v>
       </c>
-      <c r="D5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>0.41</v>
       </c>
-      <c r="D6">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="B7"/>
+      <c r="C7" t="n">
         <v>0.63</v>
       </c>
-      <c r="D7">
-        <v>2.7E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="n">
+        <v>0.027</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D8">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>0.21</v>
       </c>
-      <c r="D9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>0.16</v>
       </c>
-      <c r="D10">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>0.18</v>
       </c>
-      <c r="D11">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>0.16</v>
       </c>
-      <c r="D12">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="B13"/>
+      <c r="C13" t="n">
         <v>0.15</v>
       </c>
-      <c r="D13">
-        <v>2E-3</v>
+      <c r="D13" t="n">
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>